<commit_message>
Picked antenna for BOM and added footprint
</commit_message>
<xml_diff>
--- a/mk1/hardware/BOM.xlsx
+++ b/mk1/hardware/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\MATT\mk1\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9FF616-0ACE-4570-9968-90E0845A6B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F01FEF1-3853-4757-9B25-42FA81AB3BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1920" windowWidth="25665" windowHeight="11295" xr2:uid="{9C576334-6567-4D24-BD25-50239C784521}"/>
+    <workbookView xWindow="1965" yWindow="2265" windowWidth="25665" windowHeight="11295" xr2:uid="{9C576334-6567-4D24-BD25-50239C784521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>Item #</t>
   </si>
@@ -323,22 +323,16 @@
     <t>Antenna</t>
   </si>
   <si>
-    <t>Antenna connector</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/ProductDetail/TE-Connectivity-Linx-Technologies/CONREVSMA003.062?qs=K5ta8V%252BWhtYpGXyO%2FIVXOg%3D%3D</t>
-  </si>
-  <si>
     <t>Linx</t>
   </si>
   <si>
-    <t>CONREVSMA003.062</t>
-  </si>
-  <si>
-    <t>Edge mount</t>
-  </si>
-  <si>
-    <t>What eggtimer recommends, but only any good with a suitable antenna</t>
+    <t>https://www.mouser.co.uk/ProductDetail/TE-Connectivity-Linx-Technologies/ANT-868-PW-LP?qs=K5ta8V%252BWhtYGZ0ta3zQXkg%3D%3D</t>
+  </si>
+  <si>
+    <t>ANT-868-PW-LP</t>
+  </si>
+  <si>
+    <t>screw mount</t>
   </si>
 </sst>
 </file>
@@ -768,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302FB73F-DE7D-4142-BE74-1A53B9E320B4}">
-  <dimension ref="B2:K19"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +777,7 @@
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
     <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1101,26 +1095,24 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -1301,24 +1293,6 @@
         <v>89</v>
       </c>
       <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1338,7 +1312,7 @@
     <hyperlink ref="J15" r:id="rId14" xr:uid="{E7BFA524-D50F-4842-BEBF-1AB70F210899}"/>
     <hyperlink ref="J18" r:id="rId15" xr:uid="{F58EC075-DD00-4A56-BA64-11107B050D89}"/>
     <hyperlink ref="J17" r:id="rId16" xr:uid="{A38D392C-8B71-4F7A-AB74-B015C1B8C6CF}"/>
-    <hyperlink ref="J12" r:id="rId17" xr:uid="{86E1955C-5E2D-4978-A641-E044DB3D860A}"/>
+    <hyperlink ref="J12" r:id="rId17" xr:uid="{15B52D75-6DE5-4F61-B790-1A63E7477FEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add a few missing in and outputs, try to join up pins
</commit_message>
<xml_diff>
--- a/mk1/hardware/BOM.xlsx
+++ b/mk1/hardware/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\MATT\mk1\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F01FEF1-3853-4757-9B25-42FA81AB3BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55C6F9F-8860-413C-A60D-DBCE40B0D5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="2265" windowWidth="25665" windowHeight="11295" xr2:uid="{9C576334-6567-4D24-BD25-50239C784521}"/>
+    <workbookView xWindow="31005" yWindow="2085" windowWidth="25665" windowHeight="11295" xr2:uid="{9C576334-6567-4D24-BD25-50239C784521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>U7, U8</t>
   </si>
   <si>
-    <t>U9</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>screw mount</t>
+  </si>
+  <si>
+    <t>U9, U11, U12</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
   <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,22 +825,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -855,22 +855,22 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="K4" s="4"/>
     </row>
@@ -885,22 +885,22 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -915,22 +915,22 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" s="4"/>
     </row>
@@ -945,22 +945,22 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -975,22 +975,22 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="K8" s="4"/>
     </row>
@@ -1005,22 +1005,22 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -1029,28 +1029,28 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="I10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K10" s="4"/>
     </row>
@@ -1059,28 +1059,28 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="1"/>
     </row>
@@ -1089,28 +1089,28 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="K12" s="4"/>
     </row>
@@ -1119,28 +1119,28 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -1149,28 +1149,28 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4">
         <v>4</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K14" s="4"/>
     </row>
@@ -1179,28 +1179,28 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="K15" s="1"/>
     </row>
@@ -1209,28 +1209,28 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="G16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K16" s="4"/>
     </row>
@@ -1239,28 +1239,28 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
         <v>92</v>
       </c>
-      <c r="F17" t="s">
-        <v>93</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K17" s="1"/>
     </row>
@@ -1269,28 +1269,28 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="K18" s="4"/>
     </row>

</xml_diff>